<commit_message>
Correction in Address mapping
Signed-off-by: Wasif Adnan <mwadnan@ferroamp.se>
</commit_message>
<xml_diff>
--- a/doc/EDrive_Control_MemoryMapping.xlsx
+++ b/doc/EDrive_Control_MemoryMapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13425" yWindow="0" windowWidth="15405" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="13425" yWindow="0" windowWidth="15405" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Address Definitions" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="SignalAssign" sheetId="5" r:id="rId4"/>
     <sheet name="PMODMapping" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -350,15 +350,6 @@
     <t>SPI_CLK_DIV_1</t>
   </si>
   <si>
-    <t>0x00007FFF</t>
-  </si>
-  <si>
-    <t>0x00008000</t>
-  </si>
-  <si>
-    <t>0x000087FF</t>
-  </si>
-  <si>
     <t>Signal Assignments in top.vhd</t>
   </si>
   <si>
@@ -621,6 +612,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Each enable pin corresponds to a half bridge converter i.e. 2 PWM channels. The enable pins going to HW will correspond to the corresponding 2 PWM channels.</t>
+  </si>
+  <si>
+    <t>0x00003FFF</t>
+  </si>
+  <si>
+    <t>0x000047FF</t>
+  </si>
+  <si>
+    <t>0x00004000</t>
   </si>
 </sst>
 </file>
@@ -1088,6 +1088,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1115,6 +1116,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1130,14 +1140,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1148,13 +1155,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1454,8 +1454,8 @@
   </sheetPr>
   <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1478,10 +1478,10 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="24" t="s">
         <v>46</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>51</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>110</v>
+        <v>198</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>47</v>
@@ -1529,10 +1529,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>111</v>
+        <v>200</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>112</v>
+        <v>199</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>48</v>
@@ -1628,10 +1628,10 @@
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="32.25" customHeight="1">
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="69"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="3">
         <v>12</v>
       </c>
@@ -1641,10 +1641,10 @@
       <c r="F19" s="23"/>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="68"/>
+      <c r="C21" s="69"/>
       <c r="D21" s="7" t="s">
         <v>4</v>
       </c>
@@ -1886,7 +1886,7 @@
   </sheetPr>
   <dimension ref="A2:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -1923,20 +1923,20 @@
       <c r="A4" s="17"/>
       <c r="B4" s="18"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="72"/>
+      <c r="E4" s="73"/>
       <c r="F4" s="31"/>
       <c r="G4" s="20"/>
       <c r="H4" s="9"/>
       <c r="I4"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="73"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="42" t="s">
         <v>69</v>
       </c>
@@ -1975,10 +1975,10 @@
       <c r="E7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="70" t="s">
+      <c r="F7" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="70" t="s">
+      <c r="G7" s="71" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="9"/>
@@ -1997,8 +1997,8 @@
       <c r="E8" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:9">
@@ -2024,10 +2024,10 @@
       <c r="E10" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="74" t="s">
+      <c r="F10" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="74" t="s">
+      <c r="G10" s="75" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="9"/>
@@ -2046,8 +2046,8 @@
       <c r="E11" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:9">
@@ -2057,8 +2057,8 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="34"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:9">
@@ -2075,8 +2075,8 @@
       <c r="E13" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:9">
@@ -2102,10 +2102,10 @@
       <c r="E15" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="70" t="s">
+      <c r="F15" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="70" t="s">
+      <c r="G15" s="71" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="9"/>
@@ -2122,10 +2122,10 @@
         <v>74</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
+        <v>132</v>
+      </c>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
       <c r="H16" s="9"/>
     </row>
     <row r="17" spans="2:8">
@@ -2135,8 +2135,8 @@
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="34"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="2:8">
@@ -2151,10 +2151,10 @@
         <v>74</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
+        <v>133</v>
+      </c>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="2:8">
@@ -2222,7 +2222,7 @@
   </sheetPr>
   <dimension ref="B2:AG29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
@@ -2830,10 +2830,10 @@
         <v>22</v>
       </c>
       <c r="Y17" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z17" s="15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="AA17" s="15" t="s">
         <v>105</v>
@@ -2859,12 +2859,12 @@
     </row>
     <row r="18" spans="2:33">
       <c r="B18" s="23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="2:33">
       <c r="B19" s="23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="2:33">
@@ -2972,22 +2972,22 @@
     </row>
     <row r="24" spans="2:33" s="14" customFormat="1" ht="99.95" customHeight="1">
       <c r="B24" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="F24" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="G24" s="15" t="s">
         <v>192</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>195</v>
       </c>
       <c r="H24" s="15" t="s">
         <v>22</v>
@@ -3065,12 +3065,12 @@
         <v>44</v>
       </c>
       <c r="AG24" s="15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="2:33">
       <c r="B26" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="2:33">
@@ -3173,100 +3173,100 @@
     </row>
     <row r="29" spans="2:33" s="14" customFormat="1" ht="99.95" customHeight="1">
       <c r="B29" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E29" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="F29" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="G29" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="H29" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="I29" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="J29" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="K29" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="I29" s="15" t="s">
+      <c r="L29" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="M29" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="K29" s="15" t="s">
+      <c r="N29" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="L29" s="15" t="s">
+      <c r="O29" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="M29" s="15" t="s">
+      <c r="P29" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="N29" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="O29" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="P29" s="15" t="s">
-        <v>169</v>
-      </c>
       <c r="Q29" s="15" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="R29" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="S29" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="T29" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="U29" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="S29" s="15" t="s">
+      <c r="V29" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="T29" s="15" t="s">
+      <c r="W29" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="U29" s="15" t="s">
+      <c r="X29" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="V29" s="15" t="s">
+      <c r="Y29" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="W29" s="15" t="s">
+      <c r="Z29" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="X29" s="15" t="s">
+      <c r="AA29" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="Y29" s="15" t="s">
+      <c r="AB29" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="Z29" s="15" t="s">
+      <c r="AC29" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="AA29" s="15" t="s">
+      <c r="AD29" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="AB29" s="15" t="s">
+      <c r="AE29" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="AC29" s="15" t="s">
+      <c r="AF29" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="AD29" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="AE29" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="AF29" s="15" t="s">
-        <v>153</v>
-      </c>
       <c r="AG29" s="15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3299,7 +3299,7 @@
   <sheetData>
     <row r="2" spans="1:12" ht="18.75">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3321,11 +3321,11 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="46" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="37" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="37"/>
@@ -3353,18 +3353,18 @@
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" s="82" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
       <c r="H7" s="60"/>
       <c r="I7" s="60"/>
       <c r="J7" s="60"/>
@@ -3373,12 +3373,12 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="53"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
       <c r="H8" s="61"/>
       <c r="I8" s="61"/>
       <c r="J8" s="61"/>
@@ -3387,18 +3387,18 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="54" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" s="84" t="s">
-        <v>119</v>
-      </c>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="83" t="s">
-        <v>133</v>
-      </c>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
+        <v>115</v>
+      </c>
+      <c r="B9" s="80" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="79" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
       <c r="H9" s="61"/>
       <c r="I9" s="61"/>
       <c r="J9" s="61"/>
@@ -3407,12 +3407,12 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="53"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
       <c r="H10" s="61"/>
       <c r="I10" s="61"/>
       <c r="J10" s="61"/>
@@ -3424,17 +3424,17 @@
       <c r="B11" s="4">
         <v>0</v>
       </c>
-      <c r="C11" s="81" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" s="81"/>
+      <c r="C11" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="85"/>
       <c r="E11" s="66">
         <v>0</v>
       </c>
-      <c r="F11" s="77" t="s">
-        <v>134</v>
-      </c>
-      <c r="G11" s="78"/>
+      <c r="F11" s="81" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" s="82"/>
       <c r="H11" s="4"/>
       <c r="I11" s="9"/>
       <c r="J11" s="4"/>
@@ -3446,17 +3446,17 @@
       <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="77" t="s">
-        <v>170</v>
-      </c>
-      <c r="D12" s="78"/>
+      <c r="C12" s="81" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="82"/>
       <c r="E12" s="66">
         <v>1</v>
       </c>
-      <c r="F12" s="77" t="s">
-        <v>170</v>
-      </c>
-      <c r="G12" s="78"/>
+      <c r="F12" s="81" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" s="82"/>
       <c r="H12" s="4"/>
       <c r="I12" s="9"/>
       <c r="J12" s="4"/>
@@ -3468,17 +3468,17 @@
       <c r="B13" s="4">
         <v>2</v>
       </c>
-      <c r="C13" s="77" t="s">
-        <v>171</v>
-      </c>
-      <c r="D13" s="78"/>
+      <c r="C13" s="81" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="82"/>
       <c r="E13" s="66">
         <v>2</v>
       </c>
-      <c r="F13" s="77" t="s">
-        <v>171</v>
-      </c>
-      <c r="G13" s="78"/>
+      <c r="F13" s="81" t="s">
+        <v>168</v>
+      </c>
+      <c r="G13" s="82"/>
       <c r="H13" s="4"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -3490,17 +3490,17 @@
       <c r="B14" s="4">
         <v>3</v>
       </c>
-      <c r="C14" s="77" t="s">
-        <v>172</v>
-      </c>
-      <c r="D14" s="78"/>
+      <c r="C14" s="81" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="82"/>
       <c r="E14" s="66">
         <v>3</v>
       </c>
-      <c r="F14" s="77" t="s">
-        <v>172</v>
-      </c>
-      <c r="G14" s="78"/>
+      <c r="F14" s="81" t="s">
+        <v>169</v>
+      </c>
+      <c r="G14" s="82"/>
       <c r="H14" s="4"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -3512,17 +3512,17 @@
       <c r="B15" s="4">
         <v>4</v>
       </c>
-      <c r="C15" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15" s="78"/>
+      <c r="C15" s="81" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="82"/>
       <c r="E15" s="66">
         <v>4</v>
       </c>
-      <c r="F15" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="G15" s="78"/>
+      <c r="F15" s="81" t="s">
+        <v>170</v>
+      </c>
+      <c r="G15" s="82"/>
       <c r="H15" s="4"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -3532,11 +3532,11 @@
     <row r="16" spans="1:12" ht="15.75" thickBot="1">
       <c r="A16" s="55"/>
       <c r="B16" s="56"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="80"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="84"/>
       <c r="E16" s="57"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="80"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="84"/>
       <c r="H16" s="57"/>
       <c r="I16" s="57"/>
       <c r="J16" s="57"/>
@@ -3566,14 +3566,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B9:D9"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F11:G11"/>
@@ -3586,6 +3578,14 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F14:G14"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="800" verticalDpi="800" r:id="rId1"/>
@@ -3596,7 +3596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:Q19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -3613,48 +3613,48 @@
   <sheetData>
     <row r="2" spans="1:17" ht="21">
       <c r="A2" s="62" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="C4" s="90" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="C4" s="87" t="s">
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="J4" s="90" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="C5" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="J5" s="90" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
-      <c r="J4" s="87" t="s">
-        <v>126</v>
-      </c>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="87"/>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="C5" s="87" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="J5" s="87" t="s">
-        <v>127</v>
-      </c>
-      <c r="K5" s="87"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="87"/>
-      <c r="O5" s="87"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
     </row>
     <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="86" t="s">
-        <v>122</v>
+      <c r="A6" s="89" t="s">
+        <v>119</v>
       </c>
       <c r="C6" s="3">
         <v>7</v>
@@ -3693,86 +3693,86 @@
       <c r="O6" s="3">
         <v>12</v>
       </c>
-      <c r="Q6" s="85" t="s">
-        <v>125</v>
+      <c r="Q6" s="88" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="39.950000000000003" customHeight="1">
-      <c r="A7" s="86"/>
+      <c r="A7" s="89"/>
       <c r="C7" s="67" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="67" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="67" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="67" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7" s="63" t="s">
         <v>174</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="H7" s="63" t="s">
         <v>175</v>
-      </c>
-      <c r="E7" s="67" t="s">
-        <v>176</v>
-      </c>
-      <c r="F7" s="67" t="s">
-        <v>188</v>
-      </c>
-      <c r="G7" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="H7" s="63" t="s">
-        <v>178</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="67" t="s">
+        <v>179</v>
+      </c>
+      <c r="K7" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="L7" s="67" t="s">
+        <v>181</v>
+      </c>
+      <c r="M7" s="67" t="s">
         <v>182</v>
       </c>
-      <c r="K7" s="67" t="s">
+      <c r="N7" s="63" t="s">
+        <v>174</v>
+      </c>
+      <c r="O7" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q7" s="88"/>
+    </row>
+    <row r="8" spans="1:17" ht="39.950000000000003" customHeight="1">
+      <c r="A8" s="89"/>
+      <c r="C8" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="L7" s="67" t="s">
-        <v>184</v>
-      </c>
-      <c r="M7" s="67" t="s">
-        <v>185</v>
-      </c>
-      <c r="N7" s="63" t="s">
+      <c r="D8" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="O7" s="63" t="s">
+      <c r="F8" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="Q7" s="85"/>
-    </row>
-    <row r="8" spans="1:17" ht="39.950000000000003" customHeight="1">
-      <c r="A8" s="86"/>
-      <c r="C8" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>181</v>
-      </c>
       <c r="G8" s="63" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H8" s="63" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="M8" s="63"/>
       <c r="N8" s="63" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="O8" s="63" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q8" s="85"/>
+        <v>175</v>
+      </c>
+      <c r="Q8" s="88"/>
     </row>
     <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="86"/>
+      <c r="A9" s="89"/>
       <c r="C9" s="3">
         <v>1</v>
       </c>
@@ -3810,76 +3810,76 @@
       <c r="O9" s="3">
         <v>6</v>
       </c>
-      <c r="Q9" s="85"/>
+      <c r="Q9" s="88"/>
     </row>
     <row r="11" spans="1:17">
       <c r="C11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15.75">
-      <c r="C13" s="90" t="s">
-        <v>196</v>
+      <c r="C13" s="68" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1">
-      <c r="C14" s="89" t="s">
-        <v>200</v>
-      </c>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89"/>
+      <c r="C14" s="87" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="89"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
     </row>
     <row r="17" spans="3:6">
       <c r="C17" t="s">
-        <v>179</v>
-      </c>
-      <c r="D17" s="88" t="s">
-        <v>197</v>
-      </c>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
+        <v>176</v>
+      </c>
+      <c r="D17" s="86" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
     </row>
     <row r="18" spans="3:6">
       <c r="C18" t="s">
-        <v>180</v>
-      </c>
-      <c r="D18" s="88" t="s">
-        <v>198</v>
-      </c>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88"/>
+        <v>177</v>
+      </c>
+      <c r="D18" s="86" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
     </row>
     <row r="19" spans="3:6">
       <c r="C19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D19" s="88" t="s">
-        <v>199</v>
-      </c>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
+        <v>178</v>
+      </c>
+      <c r="D19" s="86" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J5:O5"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="C14:G15"/>
     <mergeCell ref="Q6:Q9"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="800" verticalDpi="800" r:id="rId1"/>

</xml_diff>